<commit_message>
finalise curation and render
</commit_message>
<xml_diff>
--- a/conversion_table.xlsx
+++ b/conversion_table.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C197"/>
+  <dimension ref="A1:C198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3314,6 +3314,21 @@
         <v>0</v>
       </c>
     </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>analamozaotra</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Analamazaotra</t>
+        </is>
+      </c>
+      <c r="C198">
+        <v>0.07692307692307693</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>